<commit_message>
finished first page web scraping and working on excel fill in function
</commit_message>
<xml_diff>
--- a/Air Con and Electrical (Yellow Page).xlsx
+++ b/Air Con and Electrical (Yellow Page).xlsx
@@ -1,78 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f77d448be0ee6f06/Desktop/Phone_number_scrapping/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C0289718-80B3-4D84-869D-5B064D87F5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{828D9F9B-7040-4229-AC4D-14F8DDCDE695}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{177A0FA6-C092-4816-8439-A022AEFAE3D1}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="QLD" sheetId="1" r:id="rId1"/>
-    <sheet name="NSW" sheetId="2" r:id="rId2"/>
-    <sheet name="VIC" sheetId="3" r:id="rId3"/>
-    <sheet name="SA" sheetId="5" r:id="rId4"/>
-    <sheet name="ACT" sheetId="6" r:id="rId5"/>
-    <sheet name="WA" sheetId="7" r:id="rId6"/>
-    <sheet name="NT" sheetId="8" r:id="rId7"/>
-    <sheet name="TAS" sheetId="9" r:id="rId8"/>
+    <sheet name="QLD" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NSW" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="VIC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ACT" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="WA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="NT" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TAS" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Suburb</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -91,21 +53,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -425,35 +446,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A192E7-442C-4BF5-8B3A-548E499410A9}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -462,35 +494,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91A3CC4-5FA1-475F-8938-A20F17A4CD3C}">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet2">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -499,35 +542,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C85457-0BE0-4F40-BF14-2949A0B45B09}">
-  <sheetPr codeName="Sheet3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet3">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -536,35 +590,46 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E228E0E3-19A9-40B9-8136-A3C2101D83F7}">
-  <sheetPr codeName="Sheet4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -573,35 +638,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CC7AC9-FF1A-4157-A730-EC24395C699F}">
-  <sheetPr codeName="Sheet5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet5">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -610,35 +686,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC53A846-2F5C-4095-8FB0-C5F9586EC7CA}">
-  <sheetPr codeName="Sheet6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet6">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -647,35 +734,46 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9B5D9-AD43-4D82-8335-20AEC51D3CE1}">
-  <sheetPr codeName="Sheet7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet7">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -684,8 +782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6E3B66-518D-467E-A4CD-C5EA135D2214}">
-  <sheetPr codeName="Sheet8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet8">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -693,26 +794,34 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suburb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>